<commit_message>
after bazer 7 8 2021
</commit_message>
<xml_diff>
--- a/July.xlsx
+++ b/July.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>sobji</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>dim</t>
+  </si>
+  <si>
+    <t>total bazer</t>
+  </si>
+  <si>
+    <t>Supty</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Rana</t>
+  </si>
+  <si>
+    <t>left</t>
   </si>
 </sst>
 </file>
@@ -376,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +408,7 @@
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -412,8 +427,20 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -426,13 +453,35 @@
       <c r="E2">
         <v>70</v>
       </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>110</v>
+      </c>
+      <c r="K2">
+        <v>300</v>
+      </c>
+      <c r="L2">
+        <v>214</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3">
         <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dim 7 9 2021
</commit_message>
<xml_diff>
--- a/July.xlsx
+++ b/July.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>sobji</t>
   </si>
@@ -394,7 +394,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +474,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>